<commit_message>
TestData update by shany Mohan Dhas
</commit_message>
<xml_diff>
--- a/Com_Refresh/src/test/resources/TestData.xlsx
+++ b/Com_Refresh/src/test/resources/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\MYFW\MYFW\Com_Refresh\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\OpenMrs\Com_Refresh\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -155,16 +155,16 @@
     <t>Parent,Sibling,Supervisor</t>
   </si>
   <si>
-    <t>Buttler</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>Rosie</t>
-  </si>
-  <si>
-    <t>Liam davis</t>
+    <t>Zig zag</t>
+  </si>
+  <si>
+    <t>Letin</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,7 @@
   <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,13 +615,13 @@
         <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>28</v>
@@ -741,7 +741,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>

</xml_diff>